<commit_message>
Version 5_0_1 + ShinyFMBN v3 uploaded
New and larger version of the database + significantly improved version of the app
</commit_message>
<xml_diff>
--- a/the_real_thing/FMBN_5/Excel_text_files_v5/Primers.xlsx
+++ b/the_real_thing/FMBN_5/Excel_text_files_v5/Primers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Library/CloudStorage/GoogleDrive-eugenio.parente@unibas.it/Il mio Drive/FMBN/FMBNv5/FMBN5_260324/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Library/CloudStorage/GoogleDrive-eugenio.parente@unibas.it/My Drive/FMBN/FMBNv5/FMBN5_0_1_040924/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AD95770-7A6D-1F40-883D-343479086D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D1BE9AC-3191-FA4C-8EBC-3B4E2ECE063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{0A70F4BA-8F76-A74D-83D4-A141D389E694}"/>
+    <workbookView xWindow="13580" yWindow="7900" windowWidth="26040" windowHeight="14940" xr2:uid="{AF0E3CB0-15C2-734F-B1B0-D80ED98E4E5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="246">
   <si>
     <t>primer</t>
   </si>
@@ -157,6 +157,12 @@
     <t>CCTACGGRRBGCASCAGKVRVGAAT</t>
   </si>
   <si>
+    <t>341Fm</t>
+  </si>
+  <si>
+    <t>CCTAYGGGRBGCASCAG</t>
+  </si>
+  <si>
     <t>342f</t>
   </si>
   <si>
@@ -298,6 +304,12 @@
     <t>TACNVGGGTWTCTAATCC</t>
   </si>
   <si>
+    <t>804rm</t>
+  </si>
+  <si>
+    <t>GGACTACNNGGGTATCTAAT</t>
+  </si>
+  <si>
     <t>805Rmod</t>
   </si>
   <si>
@@ -713,6 +725,54 @@
   </si>
   <si>
     <t>CCTACTGCTGCCTCCCGTAGGAGT</t>
+  </si>
+  <si>
+    <t>18SF</t>
+  </si>
+  <si>
+    <t>GTAAAAGTCGTAACAAGGTTTC</t>
+  </si>
+  <si>
+    <t>5.8S1R</t>
+  </si>
+  <si>
+    <t>GTTCAAAGAYTCGATGATTCAC</t>
+  </si>
+  <si>
+    <t>515F_III</t>
+  </si>
+  <si>
+    <t>GTGCAGCMGCCGCGGTAA</t>
+  </si>
+  <si>
+    <t>806R_III</t>
+  </si>
+  <si>
+    <t>GGACTACHTGGGTWTCTAAT</t>
+  </si>
+  <si>
+    <t>ITS3-KYO2</t>
+  </si>
+  <si>
+    <t>GATGAAGAACGYAGYRAA</t>
+  </si>
+  <si>
+    <t>ITS4F</t>
+  </si>
+  <si>
+    <t>GAACGCAGCRAAIIGYGA</t>
+  </si>
+  <si>
+    <t>ITS9R</t>
+  </si>
+  <si>
+    <t>NGS_ABCxF27</t>
+  </si>
+  <si>
+    <t>CCATCTCATCCCTGCGTGTCTCCGACTCAG</t>
+  </si>
+  <si>
+    <t>CCTCTCTATGGGCAGTCGGTGATGCWGCCTCCCGTAGGAGT</t>
   </si>
 </sst>
 </file>
@@ -1063,11 +1123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D79EFD-E646-2F4B-8040-3C5081797270}">
-  <dimension ref="A1:F122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEE9B08-6F3F-2F45-BB6C-93B68756ABA1}">
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F122"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection sqref="A1:F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,24 +1219,18 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>27</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1193,10 +1247,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1210,10 +1264,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1222,38 +1276,38 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>534</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>19</v>
@@ -1261,24 +1315,24 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
       <c r="D12">
-        <v>338</v>
+        <v>534</v>
       </c>
       <c r="E12">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -1295,7 +1349,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1312,41 +1366,41 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
       <c r="D15">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E15">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1363,10 +1417,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -1375,7 +1429,7 @@
         <v>341</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1389,49 +1443,49 @@
         <v>28</v>
       </c>
       <c r="D19">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
       </c>
       <c r="D20">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
       </c>
       <c r="D21">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="E21">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -1440,18 +1494,18 @@
         <v>28</v>
       </c>
       <c r="D22">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="E22">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1460,21 +1514,21 @@
         <v>357</v>
       </c>
       <c r="E23">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="E24">
         <v>19</v>
@@ -1482,33 +1536,33 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25">
-        <v>505</v>
+        <v>357</v>
       </c>
       <c r="E25">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>515</v>
+        <v>388</v>
       </c>
       <c r="E26">
         <v>19</v>
@@ -1516,33 +1570,27 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>232</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27">
-        <v>515</v>
-      </c>
-      <c r="E27">
-        <v>19</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D28">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="E28">
         <v>19</v>
@@ -1550,7 +1598,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
         <v>56</v>
@@ -1567,10 +1615,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -1584,10 +1632,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
@@ -1607,163 +1655,163 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E32">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D33">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E33">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
       </c>
       <c r="D34">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>234</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D35">
-        <v>534</v>
+        <v>515</v>
       </c>
       <c r="E35">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D36">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="E36">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D37">
-        <v>784</v>
+        <v>519</v>
       </c>
       <c r="E37">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D38">
-        <v>785</v>
+        <v>533</v>
       </c>
       <c r="E38">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D39">
-        <v>785</v>
+        <v>534</v>
       </c>
       <c r="E39">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
       </c>
       <c r="D40">
-        <v>785</v>
+        <v>530</v>
       </c>
       <c r="E40">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D41">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E41">
         <v>19</v>
@@ -1771,135 +1819,135 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D42">
-        <v>797</v>
+        <v>785</v>
       </c>
       <c r="E42">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D43">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="E43">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
       </c>
       <c r="D44">
-        <v>802</v>
+        <v>785</v>
       </c>
       <c r="E44">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D45">
-        <v>805</v>
+        <v>787</v>
       </c>
       <c r="E45">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
       </c>
       <c r="D46">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="E46">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D47">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="E47">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E49">
         <v>20</v>
@@ -1907,67 +1955,67 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D50">
-        <v>8</v>
+        <v>805</v>
       </c>
       <c r="E50">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D51">
-        <v>907</v>
+        <v>806</v>
       </c>
       <c r="E51">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="E52">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D53">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="E53">
         <v>20</v>
@@ -1975,47 +2023,50 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D54">
-        <v>939</v>
+        <v>806</v>
       </c>
       <c r="E54">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D55">
-        <v>939</v>
+        <v>806</v>
       </c>
       <c r="E55">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <v>8</v>
       </c>
       <c r="E56">
         <v>20</v>
@@ -2023,163 +2074,166 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D57">
-        <v>969</v>
+        <v>907</v>
       </c>
       <c r="E57">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="D58">
-        <v>1406</v>
+        <v>926</v>
       </c>
       <c r="E58">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
       </c>
       <c r="D59">
-        <v>799</v>
+        <v>926</v>
       </c>
       <c r="E59">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D60">
-        <v>806</v>
+        <v>939</v>
       </c>
       <c r="E60">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D61">
-        <v>341</v>
+        <v>939</v>
       </c>
       <c r="E61">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62">
-        <v>805</v>
+        <v>111</v>
       </c>
       <c r="E62">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>969</v>
       </c>
       <c r="E63">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>116</v>
+      </c>
+      <c r="D64">
+        <v>1406</v>
       </c>
       <c r="E64">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D65">
-        <v>27</v>
+        <v>799</v>
       </c>
       <c r="E65">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D66">
-        <v>341</v>
+        <v>806</v>
       </c>
       <c r="E66">
         <v>20</v>
@@ -2187,177 +2241,180 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C67" t="s">
         <v>28</v>
       </c>
       <c r="D67">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E67">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>805</v>
       </c>
       <c r="E68">
-        <v>37</v>
-      </c>
-      <c r="F68" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="E69">
-        <v>33</v>
-      </c>
-      <c r="F69" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
-      </c>
-      <c r="D70">
-        <v>341</v>
+        <v>15</v>
       </c>
       <c r="E70">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D71">
-        <v>806</v>
+        <v>27</v>
       </c>
       <c r="E71">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D72">
-        <v>28</v>
+        <v>341</v>
       </c>
       <c r="E72">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
       </c>
       <c r="D73">
-        <v>519</v>
+        <v>343</v>
       </c>
       <c r="E73">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>18</v>
-      </c>
-      <c r="D74">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E74">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="F74" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="E75">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="F75" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="C76" t="s">
-        <v>120</v>
+        <v>28</v>
+      </c>
+      <c r="D76">
+        <v>341</v>
       </c>
       <c r="E76">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>15</v>
+      </c>
+      <c r="D77">
+        <v>806</v>
       </c>
       <c r="E77">
         <v>22</v>
@@ -2365,159 +2422,162 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>18</v>
+      </c>
+      <c r="D78">
+        <v>28</v>
       </c>
       <c r="E78">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>28</v>
+      </c>
+      <c r="D79">
+        <v>519</v>
       </c>
       <c r="E79">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>18</v>
+      </c>
+      <c r="D80">
+        <v>27</v>
       </c>
       <c r="E80">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E81">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C82" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="E82">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E83">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E84">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="E85">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="E86">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>238</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D87">
-        <v>355</v>
+        <v>111</v>
       </c>
       <c r="E87">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
       <c r="C88" t="s">
-        <v>18</v>
-      </c>
-      <c r="D88">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="E88">
         <v>20</v>
@@ -2525,270 +2585,261 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B89" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
-      </c>
-      <c r="D89">
-        <v>341</v>
+        <v>156</v>
       </c>
       <c r="E89">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>240</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>241</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90">
-        <v>805</v>
+        <v>111</v>
       </c>
       <c r="E90">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="C91" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="E91">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B92" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="E92">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>171</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
-      </c>
-      <c r="D93">
-        <v>530</v>
+        <v>156</v>
       </c>
       <c r="E93">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>174</v>
+        <v>56</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94">
-        <v>805</v>
+        <v>28</v>
       </c>
       <c r="E94">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B95" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C95" t="s">
-        <v>28</v>
-      </c>
-      <c r="D95">
-        <v>534</v>
+        <v>15</v>
       </c>
       <c r="E95">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B96" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C96" t="s">
         <v>28</v>
       </c>
       <c r="D96">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="E96">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>244</v>
       </c>
       <c r="C97" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D97">
+        <v>27</v>
       </c>
       <c r="E97">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
-        <v>182</v>
+        <v>245</v>
       </c>
       <c r="C98" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="D98">
+        <v>355</v>
       </c>
       <c r="E98">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B99" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
       <c r="C99" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D99">
+        <v>8</v>
       </c>
       <c r="E99">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B100" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="C100" t="s">
-        <v>187</v>
+        <v>28</v>
       </c>
       <c r="D100">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E100">
-        <v>42</v>
-      </c>
-      <c r="F100" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B101" t="s">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C101" t="s">
         <v>15</v>
       </c>
+      <c r="D101">
+        <v>805</v>
+      </c>
       <c r="E101">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B102" t="s">
-        <v>191</v>
+        <v>45</v>
       </c>
       <c r="C102" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E102">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B103" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
-      </c>
-      <c r="D103">
-        <v>533</v>
+        <v>15</v>
       </c>
       <c r="E103">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B104" t="s">
-        <v>72</v>
+        <v>176</v>
       </c>
       <c r="C104" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D104">
-        <v>784</v>
+        <v>530</v>
       </c>
       <c r="E104">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
       </c>
       <c r="D105">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E105">
         <v>21</v>
@@ -2796,284 +2847,459 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B106" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
       </c>
       <c r="D106">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="E106">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B107" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C107" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D107">
-        <v>8</v>
+        <v>334</v>
       </c>
       <c r="E107">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
-        <v>36</v>
+        <v>184</v>
       </c>
       <c r="C108" t="s">
-        <v>28</v>
-      </c>
-      <c r="D108">
-        <v>341</v>
+        <v>15</v>
       </c>
       <c r="E108">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
       </c>
-      <c r="D109">
-        <v>805</v>
-      </c>
       <c r="E109">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B110" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C110" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110">
         <v>18</v>
-      </c>
-      <c r="D110">
-        <v>27</v>
-      </c>
-      <c r="E110">
-        <v>36</v>
-      </c>
-      <c r="F110" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="B111" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C111" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D111">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="E111">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F111" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>192</v>
+      </c>
+      <c r="B112" t="s">
+        <v>193</v>
+      </c>
+      <c r="C112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>194</v>
+      </c>
+      <c r="B113" t="s">
+        <v>195</v>
+      </c>
+      <c r="C113" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>196</v>
+      </c>
+      <c r="B114" t="s">
+        <v>197</v>
+      </c>
+      <c r="C114" t="s">
+        <v>28</v>
+      </c>
+      <c r="D114">
+        <v>533</v>
+      </c>
+      <c r="E114">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>198</v>
+      </c>
+      <c r="B115" t="s">
+        <v>74</v>
+      </c>
+      <c r="C115" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <v>784</v>
+      </c>
+      <c r="E115">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>199</v>
+      </c>
+      <c r="B116" t="s">
+        <v>200</v>
+      </c>
+      <c r="C116" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116">
+        <v>806</v>
+      </c>
+      <c r="E116">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>201</v>
+      </c>
+      <c r="B117" t="s">
+        <v>202</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117">
+        <v>519</v>
+      </c>
+      <c r="E117">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>203</v>
+      </c>
+      <c r="B118" t="s">
+        <v>204</v>
+      </c>
+      <c r="C118" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118">
+        <v>8</v>
+      </c>
+      <c r="E118">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>205</v>
+      </c>
+      <c r="B119" t="s">
+        <v>36</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119">
+        <v>341</v>
+      </c>
+      <c r="E119">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>206</v>
+      </c>
+      <c r="B120" t="s">
+        <v>80</v>
+      </c>
+      <c r="C120" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120">
+        <v>805</v>
+      </c>
+      <c r="E120">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>207</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B121" t="s">
         <v>208</v>
-      </c>
-      <c r="C112" t="s">
-        <v>28</v>
-      </c>
-      <c r="D112">
-        <v>338</v>
-      </c>
-      <c r="E112">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>209</v>
-      </c>
-      <c r="B113" t="s">
-        <v>210</v>
-      </c>
-      <c r="C113" t="s">
-        <v>28</v>
-      </c>
-      <c r="D113">
-        <v>340</v>
-      </c>
-      <c r="E113">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>211</v>
-      </c>
-      <c r="B114" t="s">
-        <v>212</v>
-      </c>
-      <c r="C114" t="s">
-        <v>213</v>
-      </c>
-      <c r="D114">
-        <v>1492</v>
-      </c>
-      <c r="E114">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>214</v>
-      </c>
-      <c r="B115" t="s">
-        <v>215</v>
-      </c>
-      <c r="C115" t="s">
-        <v>28</v>
-      </c>
-      <c r="D115">
-        <v>344</v>
-      </c>
-      <c r="E115">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>216</v>
-      </c>
-      <c r="B116" t="s">
-        <v>217</v>
-      </c>
-      <c r="C116" t="s">
-        <v>28</v>
-      </c>
-      <c r="E116">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>218</v>
-      </c>
-      <c r="B117" t="s">
-        <v>72</v>
-      </c>
-      <c r="C117" t="s">
-        <v>15</v>
-      </c>
-      <c r="D117">
-        <v>812</v>
-      </c>
-      <c r="E117">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>219</v>
-      </c>
-      <c r="B118" t="s">
-        <v>220</v>
-      </c>
-      <c r="C118" t="s">
-        <v>15</v>
-      </c>
-      <c r="E118">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>221</v>
-      </c>
-      <c r="B119" t="s">
-        <v>76</v>
-      </c>
-      <c r="C119" t="s">
-        <v>15</v>
-      </c>
-      <c r="E119">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>12</v>
-      </c>
-      <c r="B120" t="s">
-        <v>191</v>
-      </c>
-      <c r="C120" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>222</v>
-      </c>
-      <c r="B121" t="s">
-        <v>223</v>
       </c>
       <c r="C121" t="s">
         <v>18</v>
       </c>
       <c r="D121">
+        <v>27</v>
+      </c>
+      <c r="E121">
+        <v>36</v>
+      </c>
+      <c r="F121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>209</v>
+      </c>
+      <c r="B122" t="s">
+        <v>210</v>
+      </c>
+      <c r="C122" t="s">
+        <v>191</v>
+      </c>
+      <c r="D122">
+        <v>354</v>
+      </c>
+      <c r="E122">
+        <v>34</v>
+      </c>
+      <c r="F122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>211</v>
+      </c>
+      <c r="B123" t="s">
+        <v>212</v>
+      </c>
+      <c r="C123" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123">
+        <v>338</v>
+      </c>
+      <c r="E123">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>213</v>
+      </c>
+      <c r="B124" t="s">
+        <v>214</v>
+      </c>
+      <c r="C124" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124">
+        <v>340</v>
+      </c>
+      <c r="E124">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>215</v>
+      </c>
+      <c r="B125" t="s">
+        <v>216</v>
+      </c>
+      <c r="C125" t="s">
+        <v>217</v>
+      </c>
+      <c r="D125">
+        <v>1492</v>
+      </c>
+      <c r="E125">
         <v>20</v>
       </c>
-      <c r="E121">
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126" t="s">
+        <v>219</v>
+      </c>
+      <c r="C126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D126">
+        <v>344</v>
+      </c>
+      <c r="E126">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>220</v>
+      </c>
+      <c r="B127" t="s">
+        <v>221</v>
+      </c>
+      <c r="C127" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>222</v>
+      </c>
+      <c r="B128" t="s">
+        <v>74</v>
+      </c>
+      <c r="C128" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128">
+        <v>812</v>
+      </c>
+      <c r="E128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>223</v>
+      </c>
+      <c r="B129" t="s">
+        <v>224</v>
+      </c>
+      <c r="C129" t="s">
+        <v>15</v>
+      </c>
+      <c r="E129">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>225</v>
+      </c>
+      <c r="B130" t="s">
+        <v>78</v>
+      </c>
+      <c r="C130" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" t="s">
+        <v>195</v>
+      </c>
+      <c r="C131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>226</v>
+      </c>
+      <c r="B132" t="s">
+        <v>227</v>
+      </c>
+      <c r="C132" t="s">
+        <v>18</v>
+      </c>
+      <c r="D132">
+        <v>20</v>
+      </c>
+      <c r="E132">
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>224</v>
-      </c>
-      <c r="B122" t="s">
-        <v>225</v>
-      </c>
-      <c r="C122" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>228</v>
+      </c>
+      <c r="B133" t="s">
+        <v>229</v>
+      </c>
+      <c r="C133" t="s">
+        <v>28</v>
+      </c>
+      <c r="D133">
         <v>361</v>
       </c>
-      <c r="E122">
+      <c r="E133">
         <v>24</v>
       </c>
     </row>

</xml_diff>